<commit_message>
out of game - hierarchy
</commit_message>
<xml_diff>
--- a/EPokerTestData.xlsx
+++ b/EPokerTestData.xlsx
@@ -6,13 +6,14 @@
   </bookViews>
   <sheets>
     <sheet name="TestSchema" sheetId="1" r:id="rId1"/>
+    <sheet name="Test2Schema" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>GDE_FIELD_NAMES</t>
   </si>
@@ -20,16 +21,64 @@
     <t>TestInt</t>
   </si>
   <si>
+    <t>TestString</t>
+  </si>
+  <si>
+    <t>TestList</t>
+  </si>
+  <si>
+    <t>TestSchema</t>
+  </si>
+  <si>
     <t>GDE_FIELD_TYPES</t>
   </si>
   <si>
     <t>int</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>list_string</t>
+  </si>
+  <si>
+    <t>Test2Schema</t>
+  </si>
+  <si>
     <t>TestSchema001</t>
   </si>
   <si>
+    <t>Hello World!</t>
+  </si>
+  <si>
+    <t>"Hello","World"</t>
+  </si>
+  <si>
+    <t>Test2Schema001</t>
+  </si>
+  <si>
     <t>TestSchema002</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>TestBool</t>
+  </si>
+  <si>
+    <t>TestIntList</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>list_int</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
   </si>
 </sst>
 </file>
@@ -75,7 +124,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -88,29 +137,111 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0">
         <v>1</v>
       </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0">
         <v>2</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="0" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>